<commit_message>
Black Scholes with setting parameters in Variables environment
</commit_message>
<xml_diff>
--- a/HelperFiles/OptionPrice.xlsx
+++ b/HelperFiles/OptionPrice.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/krzysiekbienias/Downloads/ControlFiles/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/krzysiekbienias/Library/Mobile Documents/com~apple~CloudDocs/Documents/GitHub/BlackScholesWorld/HelperFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBE0268E-F32A-AB40-8C59-FCB0E062DF20}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A08719DF-C12C-E745-80BD-FE295C8EDF4B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="3" xr2:uid="{E6780EDD-42FF-9C43-8308-9E99EAAA7968}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16740" activeTab="1" xr2:uid="{E6780EDD-42FF-9C43-8308-9E99EAAA7968}"/>
   </bookViews>
   <sheets>
     <sheet name="Input 10D" sheetId="4" r:id="rId1"/>
-    <sheet name="Input 3M" sheetId="3" r:id="rId2"/>
+    <sheet name="Input_3M" sheetId="3" r:id="rId2"/>
     <sheet name="Input 6M" sheetId="1" r:id="rId3"/>
     <sheet name="Scenario Generator" sheetId="5" r:id="rId4"/>
     <sheet name="Dynamic For Report" sheetId="7" r:id="rId5"/>
@@ -25,12 +25,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -898,8 +892,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F9A4FCF-F524-0045-8F19-D207ABEB0014}">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1343,7 +1337,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7718147-768E-6D44-9A47-92DA3BFA74FC}">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>

</xml_diff>